<commit_message>
Join entre Individual e Pizza
</commit_message>
<xml_diff>
--- a/Teste_1_Jogador_Completo/Sumula_Novo_Padrao.xlsx
+++ b/Teste_1_Jogador_Completo/Sumula_Novo_Padrao.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Roberto\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Roberto\Documents\Baygon Geral\Codigo\associacao-futebol\Teste_1_Jogador_Completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59DECE78-700C-46D5-A7BC-1DC87261E018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA754D7-C693-4988-ABDE-5CE13E713912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,8 +22,6 @@
     <sheet name="Defesas" sheetId="9" r:id="rId7"/>
     <sheet name="Ouros" sheetId="6" r:id="rId8"/>
     <sheet name="Contra" sheetId="7" r:id="rId9"/>
-    <sheet name="Colaboracao" sheetId="8" r:id="rId10"/>
-    <sheet name="Copa" sheetId="10" r:id="rId11"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="68">
   <si>
     <t>Boleiro</t>
   </si>
@@ -221,6 +219,24 @@
   </si>
   <si>
     <t>Defesas de Penalti</t>
+  </si>
+  <si>
+    <t>Atacante</t>
+  </si>
+  <si>
+    <t>Ala</t>
+  </si>
+  <si>
+    <t>Zagueiro</t>
+  </si>
+  <si>
+    <t>Goleiro</t>
+  </si>
+  <si>
+    <t>Meia</t>
+  </si>
+  <si>
+    <t>Baba - Geral</t>
   </si>
 </sst>
 </file>
@@ -262,12 +278,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -548,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0CE5C4D-E381-4C77-8E58-F0981655C7F9}">
-  <dimension ref="A2:C6"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -563,6 +578,11 @@
     <col min="6" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>67</v>
+      </c>
+    </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
@@ -624,82 +644,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2A69FDC-6EF2-424D-8AAD-931022E6FFFC}">
-  <dimension ref="A1:C2"/>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF202CB4-8283-47F3-9B3C-9799944001BB}">
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F4B109D-249F-4716-BB18-9AAFF8024B22}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF202CB4-8283-47F3-9B3C-9799944001BB}">
-  <dimension ref="A1:B2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,6 +667,110 @@
         <v>60</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
@@ -724,13 +778,13 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O45"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -740,10 +794,10 @@
     <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="14.7109375" customWidth="1"/>
     <col min="12" max="12" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -754,15 +808,8 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -800,16 +847,13 @@
         <v>8</v>
       </c>
       <c r="M2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N2" t="s">
-        <v>18</v>
-      </c>
-      <c r="O2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -853,11 +897,8 @@
       <c r="N3">
         <v>0</v>
       </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -883,7 +924,7 @@
         <v>1</v>
       </c>
       <c r="I4">
-        <f t="shared" ref="I4:I39" si="0" xml:space="preserve"> SUM(1,D4,E4,(F4*3),H4)</f>
+        <f t="shared" ref="I4:I37" si="0" xml:space="preserve"> SUM(1,D4,E4,(F4*3),H4)</f>
         <v>22</v>
       </c>
       <c r="J4">
@@ -901,11 +942,8 @@
       <c r="N4">
         <v>0</v>
       </c>
-      <c r="O4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -944,16 +982,13 @@
         <v>0</v>
       </c>
       <c r="M5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>1</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -997,11 +1032,8 @@
       <c r="N6">
         <v>0</v>
       </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -1045,11 +1077,8 @@
       <c r="N7">
         <v>0</v>
       </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1093,11 +1122,8 @@
       <c r="N8">
         <v>0</v>
       </c>
-      <c r="O8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -1141,11 +1167,8 @@
       <c r="N9">
         <v>0</v>
       </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
@@ -1189,11 +1212,8 @@
       <c r="N10">
         <v>0</v>
       </c>
-      <c r="O10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1237,11 +1257,8 @@
       <c r="N11">
         <v>0</v>
       </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1285,11 +1302,8 @@
       <c r="N12">
         <v>0</v>
       </c>
-      <c r="O12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1333,11 +1347,8 @@
       <c r="N13">
         <v>0</v>
       </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1381,11 +1392,8 @@
       <c r="N14">
         <v>0</v>
       </c>
-      <c r="O14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>12</v>
       </c>
@@ -1429,11 +1437,8 @@
       <c r="N15">
         <v>0</v>
       </c>
-      <c r="O15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>12</v>
       </c>
@@ -1477,11 +1482,8 @@
       <c r="N16">
         <v>0</v>
       </c>
-      <c r="O16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -1525,11 +1527,8 @@
       <c r="N17">
         <v>0</v>
       </c>
-      <c r="O17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>12</v>
       </c>
@@ -1573,11 +1572,8 @@
       <c r="N18">
         <v>0</v>
       </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>12</v>
       </c>
@@ -1616,16 +1612,13 @@
         <v>0</v>
       </c>
       <c r="M19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N19">
         <v>0</v>
       </c>
-      <c r="O19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -1667,13 +1660,10 @@
         <v>0</v>
       </c>
       <c r="N20">
-        <v>0</v>
-      </c>
-      <c r="O20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>12</v>
       </c>
@@ -1717,11 +1707,8 @@
       <c r="N21">
         <v>0</v>
       </c>
-      <c r="O21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>12</v>
       </c>
@@ -1765,11 +1752,8 @@
       <c r="N22">
         <v>0</v>
       </c>
-      <c r="O22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1813,11 +1797,8 @@
       <c r="N23">
         <v>0</v>
       </c>
-      <c r="O23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -1861,11 +1842,8 @@
       <c r="N24">
         <v>0</v>
       </c>
-      <c r="O24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1904,16 +1882,13 @@
         <v>0</v>
       </c>
       <c r="M25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N25">
-        <v>1</v>
-      </c>
-      <c r="O25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1957,11 +1932,8 @@
       <c r="N26">
         <v>0</v>
       </c>
-      <c r="O26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -2005,11 +1977,8 @@
       <c r="N27">
         <v>0</v>
       </c>
-      <c r="O27">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -2048,16 +2017,13 @@
         <v>0</v>
       </c>
       <c r="M28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N28">
         <v>0</v>
       </c>
-      <c r="O28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -2101,11 +2067,8 @@
       <c r="N29">
         <v>0</v>
       </c>
-      <c r="O29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>13</v>
       </c>
@@ -2144,16 +2107,13 @@
         <v>0</v>
       </c>
       <c r="M30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N30">
         <v>0</v>
       </c>
-      <c r="O30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -2197,11 +2157,8 @@
       <c r="N31">
         <v>0</v>
       </c>
-      <c r="O31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>13</v>
       </c>
@@ -2240,16 +2197,13 @@
         <v>0</v>
       </c>
       <c r="M32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N32">
         <v>0</v>
       </c>
-      <c r="O32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>14</v>
       </c>
@@ -2293,11 +2247,8 @@
       <c r="N33">
         <v>0</v>
       </c>
-      <c r="O33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>14</v>
       </c>
@@ -2336,16 +2287,13 @@
         <v>0</v>
       </c>
       <c r="M34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N34">
-        <v>1</v>
-      </c>
-      <c r="O34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>14</v>
       </c>
@@ -2384,16 +2332,13 @@
         <v>0</v>
       </c>
       <c r="M35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N35">
-        <v>0</v>
-      </c>
-      <c r="O35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
@@ -2435,13 +2380,10 @@
         <v>0</v>
       </c>
       <c r="N36">
-        <v>0</v>
-      </c>
-      <c r="O36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>14</v>
       </c>
@@ -2485,11 +2427,8 @@
       <c r="N37">
         <v>0</v>
       </c>
-      <c r="O37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2533,11 +2472,8 @@
       <c r="N38">
         <v>0</v>
       </c>
-      <c r="O38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -2576,16 +2512,13 @@
         <v>20</v>
       </c>
       <c r="M39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N39">
         <v>0</v>
       </c>
-      <c r="O39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>14</v>
       </c>
@@ -2629,11 +2562,8 @@
       <c r="N40">
         <v>0</v>
       </c>
-      <c r="O40">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -2677,11 +2607,8 @@
       <c r="N41">
         <v>0</v>
       </c>
-      <c r="O41">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -2725,11 +2652,8 @@
       <c r="N42">
         <v>0</v>
       </c>
-      <c r="O42">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
@@ -2773,11 +2697,8 @@
       <c r="N43">
         <v>0</v>
       </c>
-      <c r="O43">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
@@ -2821,11 +2742,8 @@
       <c r="N44">
         <v>0</v>
       </c>
-      <c r="O44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>14</v>
       </c>
@@ -2853,6 +2771,21 @@
       <c r="I45">
         <f xml:space="preserve"> SUM(1,D45,E45,(F45*3),H45)</f>
         <v>3</v>
+      </c>
+      <c r="J45">
+        <v>0</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>0</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2869,7 +2802,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2878,13 +2811,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3050,7 +2979,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3105,6 +3034,9 @@
       </c>
       <c r="B6" t="s">
         <v>20</v>
+      </c>
+      <c r="C6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3121,7 +3053,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3319,7 +3251,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3353,7 +3285,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="A1:C3"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Definição de Nomes para Validação de Dados
</commit_message>
<xml_diff>
--- a/Teste_1_Jogador_Completo/Sumula_Novo_Padrao.xlsx
+++ b/Teste_1_Jogador_Completo/Sumula_Novo_Padrao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Roberto\Documents\Baygon Geral\Codigo\associacao-futebol\Teste_1_Jogador_Completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DA754D7-C693-4988-ABDE-5CE13E713912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8DA002-B35E-48E8-B080-BE1F30EF55AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,6 +23,10 @@
     <sheet name="Ouros" sheetId="6" r:id="rId8"/>
     <sheet name="Contra" sheetId="7" r:id="rId9"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Boleiros!$A$2:$B$2</definedName>
+    <definedName name="BoleirosRegistrados" comment="Todo boleiro deve ser registrado aqui para poder ser inserido nas outras abas">Boleiros!$A$3:$A$15</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="68">
   <si>
     <t>Boleiro</t>
   </si>
@@ -566,7 +570,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,7 +653,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,7 +673,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="B3" t="s">
         <v>62</v>
@@ -677,39 +681,39 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="B4" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B8" t="s">
         <v>62</v>
@@ -717,15 +721,15 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B9" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>64</v>
@@ -733,7 +737,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="B11" t="s">
         <v>66</v>
@@ -749,26 +753,26 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B14" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -781,10 +785,10 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N31" sqref="N31"/>
+      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -857,8 +861,9 @@
       <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" t="s">
-        <v>9</v>
+      <c r="B3" t="str">
+        <f>BoleirosRegistrados</f>
+        <v>Anderson</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -2793,6 +2798,18 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B32" xr:uid="{3DD5FD61-9509-4B3D-AB14-EC7C2E4743F0}">
+      <formula1>BoleirosRegistrados</formula1>
+    </dataValidation>
+    <dataValidation allowBlank="1" showInputMessage="1" sqref="D46" xr:uid="{E90E8BDC-2ADA-455F-B467-A547CABD99FD}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="É necessário registrar o boleiro na aba &quot;Boleiros&quot;" sqref="B33:B45 B47:B1048576" xr:uid="{01FBB186-CE36-4D02-9B13-CF4FA88B6601}">
+      <formula1>BoleirosRegistrados</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="Caso seja um novo boleiro, necessário registrá-lo na aba &quot;Boleiros&quot;" sqref="B46" xr:uid="{0502E18F-6C34-47DD-96A9-F4161414C441}">
+      <formula1>BoleirosRegistrados</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3052,8 +3069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E964FD9E-4A6A-4EAB-8156-272A1DF29334}">
   <dimension ref="A1:D22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3242,6 +3259,11 @@
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="Caso seja um novo boleiro, necessário registrá-lo na aba &quot;Boleiros&quot;" sqref="C3:D1048576" xr:uid="{19159622-F538-4F4C-99F1-822D56EB37BB}">
+      <formula1>BoleirosRegistrados</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -3251,7 +3273,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B3" sqref="B3:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3276,6 +3298,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="Caso seja um novo boleiro, necessário registrá-lo na aba &quot;Boleiros&quot;" sqref="B3:B1048576" xr:uid="{DB21C9C4-68E5-4E24-9F3D-4FABECD9A3FD}">
+      <formula1>BoleirosRegistrados</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -3285,7 +3312,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="B3" sqref="B3:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3307,6 +3334,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="Caso seja um novo boleiro, necessário registrá-lo na aba &quot;Boleiros&quot;" sqref="B3:B1048576" xr:uid="{5BC51B03-AC10-4445-B4CC-D6E5DF068C60}">
+      <formula1>BoleirosRegistrados</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -3316,7 +3348,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3341,6 +3373,11 @@
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="Caso seja um novo boleiro, necessário registrá-lo na aba &quot;Boleiros&quot;" sqref="B3:B1048576" xr:uid="{8A2FB513-E0C8-4FD6-9546-F84A1D316E48}">
+      <formula1>BoleirosRegistrados</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Lista para Validação de Dados atualizada dinamicamente
</commit_message>
<xml_diff>
--- a/Teste_1_Jogador_Completo/Sumula_Novo_Padrao.xlsx
+++ b/Teste_1_Jogador_Completo/Sumula_Novo_Padrao.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\José Roberto\Documents\Baygon Geral\Codigo\associacao-futebol\Teste_1_Jogador_Completo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A8DA002-B35E-48E8-B080-BE1F30EF55AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3546D7-9ABF-4781-83E5-03C2A7BDF25E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" tabRatio="753" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Boleiros!$A$2:$B$2</definedName>
-    <definedName name="BoleirosRegistrados" comment="Todo boleiro deve ser registrado aqui para poder ser inserido nas outras abas">Boleiros!$A$3:$A$15</definedName>
+    <definedName name="BoleirosRegistrados" comment="Todo boleiro deve ser registrado aqui para poder ser inserido nas outras abas">OFFSET(Boleiros!$A$2, 0, 0, COUNTA(Boleiros!$A:$A)-1, 1)</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -570,7 +570,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -653,7 +653,7 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -785,10 +785,10 @@
   <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C50" sqref="C50"/>
+      <selection pane="bottomRight" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,7 +862,7 @@
         <v>11</v>
       </c>
       <c r="B3" t="str">
-        <f>BoleirosRegistrados</f>
+        <f ca="1">BoleirosRegistrados</f>
         <v>Anderson</v>
       </c>
       <c r="C3" t="s">
@@ -2798,15 +2798,9 @@
     <mergeCell ref="A1:H1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B3:B32" xr:uid="{3DD5FD61-9509-4B3D-AB14-EC7C2E4743F0}">
-      <formula1>BoleirosRegistrados</formula1>
-    </dataValidation>
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" sqref="D46" xr:uid="{E90E8BDC-2ADA-455F-B467-A547CABD99FD}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="É necessário registrar o boleiro na aba &quot;Boleiros&quot;" sqref="B33:B45 B47:B1048576" xr:uid="{01FBB186-CE36-4D02-9B13-CF4FA88B6601}">
-      <formula1>BoleirosRegistrados</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="Caso seja um novo boleiro, necessário registrá-lo na aba &quot;Boleiros&quot;" sqref="B46" xr:uid="{0502E18F-6C34-47DD-96A9-F4161414C441}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Boleiro Inválido" error="Caso seja um novo boleiro, necessário registrá-lo na aba &quot;Boleiros&quot;" sqref="B3:B1048576" xr:uid="{0502E18F-6C34-47DD-96A9-F4161414C441}">
       <formula1>BoleirosRegistrados</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>